<commit_message>
API Khám Bệnh + CDDV
</commit_message>
<xml_diff>
--- a/DataTest/Data_API_Tiếp_nhận.xlsx
+++ b/DataTest/Data_API_Tiếp_nhận.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HIS api automation\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38212FA1-DF73-4B81-ADB3-FE4879862407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6397EF-49F6-402D-9CA6-B3043276F92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="18984" windowHeight="8880" xr2:uid="{6E887C13-9AED-47A6-9E45-95980517E124}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E887C13-9AED-47A6-9E45-95980517E124}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,7 +260,7 @@
     <t>Thẻ BHYT hợp lệ</t>
   </si>
   <si>
-    <t>DN4127389127610</t>
+    <t>DN4127389127641</t>
   </si>
 </sst>
 </file>
@@ -637,7 +637,7 @@
   <dimension ref="A1:BH7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -871,7 +871,7 @@
     </row>
     <row r="2" spans="1:60">
       <c r="A2">
-        <v>138</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -883,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>46200020923</v>
+        <v>46200020983</v>
       </c>
       <c r="F2">
         <v>356572156</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="3" spans="1:60">
       <c r="A3">
-        <v>139</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -1026,7 +1026,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>46200020924</v>
+        <v>46200020984</v>
       </c>
       <c r="F3">
         <v>356572156</v>

</xml_diff>

<commit_message>
Done tự động generate khám bệnh + CDDV
</commit_message>
<xml_diff>
--- a/DataTest/Data_API_Tiếp_nhận.xlsx
+++ b/DataTest/Data_API_Tiếp_nhận.xlsx
@@ -737,7 +737,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>901</v>
+        <v>985</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>46200501595</v>
+        <v>46200501679</v>
       </c>
       <c r="F2" t="n">
         <v>356572156</v>
@@ -825,7 +825,7 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>DN4127450128106</t>
+          <t>DN4127450128190</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -929,7 +929,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>902</v>
+        <v>986</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>46200501596</v>
+        <v>46200501680</v>
       </c>
       <c r="F3" t="n">
         <v>356572156</v>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>DN4127450128107</t>
+          <t>DN4127450128191</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
@@ -1121,7 +1121,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>903</v>
+        <v>987</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>46200501597</v>
+        <v>46200501681</v>
       </c>
       <c r="F4" t="n">
         <v>356572156</v>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>DN4127450128108</t>
+          <t>DN4127450128192</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -1313,7 +1313,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>904</v>
+        <v>988</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1329,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>46200501598</v>
+        <v>46200501682</v>
       </c>
       <c r="F5" t="n">
         <v>356572156</v>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>DN4127450128109</t>
+          <t>DN4127450128193</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
@@ -1505,7 +1505,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>905</v>
+        <v>989</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1521,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>46200501599</v>
+        <v>46200501683</v>
       </c>
       <c r="F6" t="n">
         <v>356572156</v>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>DN4127450128110</t>
+          <t>DN4127450128194</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">

</xml_diff>

<commit_message>
Done tự động generate Cận Lâm Sàng
</commit_message>
<xml_diff>
--- a/DataTest/Data_API_Tiếp_nhận.xlsx
+++ b/DataTest/Data_API_Tiếp_nhận.xlsx
@@ -737,7 +737,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1702</v>
+        <v>1810</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -753,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>46200502396</v>
+        <v>46200602503</v>
       </c>
       <c r="F2" t="n">
         <v>356572156</v>
@@ -825,7 +825,7 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>DN4127450128907</t>
+          <t>DN4127460129014</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -929,7 +929,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1703</v>
+        <v>1811</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>46200502397</v>
+        <v>46200602504</v>
       </c>
       <c r="F3" t="n">
         <v>356572156</v>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>DN4127450128908</t>
+          <t>DN4127460129015</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">

</xml_diff>

<commit_message>
Cải tiến Tiếp nhận
</commit_message>
<xml_diff>
--- a/DataTest/Data_API_Tiếp_nhận.xlsx
+++ b/DataTest/Data_API_Tiếp_nhận.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH3"/>
+  <dimension ref="A1:BH5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -737,7 +738,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1844</v>
+        <v>1906</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -753,7 +754,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>46200602537</v>
+        <v>46200602599</v>
       </c>
       <c r="F2" t="n">
         <v>356572156</v>
@@ -798,7 +799,6 @@
           <t>Công Ty OPTIMA POWER TOOLS Việt Nam</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
         <v>1</v>
       </c>
@@ -825,7 +825,7 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>DN4127460129048</t>
+          <t>DN4127460129099</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -852,14 +852,12 @@
       <c r="AD2" t="n">
         <v>0</v>
       </c>
-      <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="b">
         <v>0</v>
       </c>
       <c r="AG2" t="b">
         <v>0</v>
       </c>
-      <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="n">
         <v>24</v>
       </c>
@@ -878,7 +876,6 @@
       <c r="AN2" t="n">
         <v>80</v>
       </c>
-      <c r="AO2" t="inlineStr"/>
       <c r="AP2" t="n">
         <v>3839</v>
       </c>
@@ -907,29 +904,20 @@
       <c r="AW2" t="n">
         <v>560</v>
       </c>
-      <c r="AX2" t="inlineStr"/>
-      <c r="AY2" t="inlineStr"/>
-      <c r="AZ2" t="inlineStr"/>
       <c r="BA2" t="inlineStr">
         <is>
           <t>||149|09/05/2024 09:13||||||3839||||New|4803|80|||2|1083660|||</t>
         </is>
       </c>
-      <c r="BB2" t="inlineStr"/>
-      <c r="BC2" t="inlineStr"/>
-      <c r="BD2" t="inlineStr"/>
-      <c r="BE2" t="inlineStr"/>
       <c r="BF2" t="inlineStr">
         <is>
           <t>||1|Normal|CorrectRoute|09/05/2024 09:13|3266971|Quách Bảo Hưng 82|24|Male|01/01/2000 00:00|5/49 Ntl|765|26926|01|VN|134||DN4127389127512|2|80|None|||||||||3839|Open|||||||||||149|09/05/2024 09:13||||||3839||||New|4803|80|||2|1083660|||</t>
         </is>
       </c>
-      <c r="BG2" t="inlineStr"/>
-      <c r="BH2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1845</v>
+        <v>1907</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -945,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>46200602538</v>
+        <v>46200602600</v>
       </c>
       <c r="F3" t="n">
         <v>356572156</v>
@@ -990,7 +978,6 @@
           <t>Công Ty OPTIMA POWER TOOLS Việt Nam</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="n">
         <v>1</v>
       </c>
@@ -1015,43 +1002,15 @@
           <t>5/49 Ntl</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>DN4127460129049</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>BHXH</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>2024-01-01T00:00:00+07:00</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>2025-01-01T00:00:00+07:00</t>
-        </is>
-      </c>
-      <c r="AB3" t="n">
-        <v>3075</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>1</v>
-      </c>
       <c r="AD3" t="n">
         <v>0</v>
       </c>
-      <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="b">
         <v>0</v>
       </c>
       <c r="AG3" t="b">
         <v>0</v>
       </c>
-      <c r="AH3" t="inlineStr"/>
       <c r="AI3" t="n">
         <v>24</v>
       </c>
@@ -1065,20 +1024,14 @@
         <v>1</v>
       </c>
       <c r="AM3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN3" t="n">
-        <v>80</v>
-      </c>
-      <c r="AO3" t="inlineStr"/>
+        <v>0</v>
+      </c>
       <c r="AP3" t="n">
         <v>3839</v>
       </c>
-      <c r="AQ3" t="inlineStr">
-        <is>
-          <t>Thẻ BHYT hợp lệ</t>
-        </is>
-      </c>
       <c r="AR3" t="n">
         <v>1</v>
       </c>
@@ -1099,25 +1052,482 @@
       <c r="AW3" t="n">
         <v>560</v>
       </c>
-      <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="inlineStr"/>
-      <c r="AZ3" t="inlineStr"/>
       <c r="BA3" t="inlineStr">
         <is>
           <t>||149|09/05/2024 09:13||||||3839||||New|4803|80|||2|1083660|||</t>
         </is>
       </c>
-      <c r="BB3" t="inlineStr"/>
-      <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="inlineStr"/>
-      <c r="BE3" t="inlineStr"/>
       <c r="BF3" t="inlineStr">
         <is>
           <t>||1|Normal|CorrectRoute|09/05/2024 09:13|3266971|Quách Bảo Hưng 82|24|Male|01/01/2000 00:00|5/49 Ntl|765|26926|01|VN|134||DN4127389127512|2|80|None|||||||||3839|Open|||||||||||149|09/05/2024 09:13||||||3839||||New|4803|80|||2|1083660|||</t>
         </is>
       </c>
-      <c r="BG3" t="inlineStr"/>
-      <c r="BH3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1908</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Quách Bảo Hưng</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2000-01-01T00:00:00+07:00</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>46200602601</v>
+      </c>
+      <c r="F4" t="n">
+        <v>356572156</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>79</v>
+      </c>
+      <c r="K4" t="n">
+        <v>765</v>
+      </c>
+      <c r="L4" t="n">
+        <v>26926</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>5/49 Ntl</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>134</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Công Ty OPTIMA POWER TOOLS Việt Nam</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Công Ty OPTIMA POWER TOOLS Việt Nam</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Quách Bảo Minh Phúc 2</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>5/49 Ntl, Phường 07, Quận Bình Thạnh, Thành phố Hồ Chí Minh</t>
+        </is>
+      </c>
+      <c r="U4" t="n">
+        <v>546378305</v>
+      </c>
+      <c r="V4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>5/49 Ntl</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>DN4127460129101</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>BHXH</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>2024-01-01T00:00:00+07:00</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>2025-01-01T00:00:00+07:00</t>
+        </is>
+      </c>
+      <c r="AB4" t="n">
+        <v>3075</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>80</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>3839</v>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t>Thẻ BHYT hợp lệ</t>
+        </is>
+      </c>
+      <c r="AR4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>4803</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>149</v>
+      </c>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>2024-05-09T09:13:34.2378979+07:00</t>
+        </is>
+      </c>
+      <c r="AV4" t="n">
+        <v>1094172</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>560</v>
+      </c>
+      <c r="BA4" t="inlineStr">
+        <is>
+          <t>||149|09/05/2024 09:13||||||3839||||New|4803|80|||2|1083660|||</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>||1|Normal|CorrectRoute|09/05/2024 09:13|3266971|Quách Bảo Hưng 82|24|Male|01/01/2000 00:00|5/49 Ntl|765|26926|01|VN|134||DN4127389127512|2|80|None|||||||||3839|Open|||||||||||149|09/05/2024 09:13||||||3839||||New|4803|80|||2|1083660|||</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1909</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Quách Bảo Hưng</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2000-01-01T00:00:00+07:00</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>46200602602</v>
+      </c>
+      <c r="F5" t="n">
+        <v>356572156</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>79</v>
+      </c>
+      <c r="K5" t="n">
+        <v>765</v>
+      </c>
+      <c r="L5" t="n">
+        <v>26926</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>5/49 Ntl</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>134</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Công Ty OPTIMA POWER TOOLS Việt Nam</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Công Ty OPTIMA POWER TOOLS Việt Nam</t>
+        </is>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Quách Bảo Minh Phúc 2</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>5/49 Ntl, Phường 07, Quận Bình Thạnh, Thành phố Hồ Chí Minh</t>
+        </is>
+      </c>
+      <c r="U5" t="n">
+        <v>546378305</v>
+      </c>
+      <c r="V5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>5/49 Ntl</t>
+        </is>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>24</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>3839</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>4803</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>149</v>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>2024-05-09T09:13:34.2378979+07:00</t>
+        </is>
+      </c>
+      <c r="AV5" t="n">
+        <v>1094172</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>560</v>
+      </c>
+      <c r="BA5" t="inlineStr">
+        <is>
+          <t>||149|09/05/2024 09:13||||||3839||||New|4803|80|||2|1083660|||</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>||1|Normal|CorrectRoute|09/05/2024 09:13|3266971|Quách Bảo Hưng 82|24|Male|01/01/2000 00:00|5/49 Ntl|765|26926|01|VN|134||DN4127389127512|2|80|None|||||||||3839|Open|||||||||||149|09/05/2024 09:13||||||3839||||New|4803|80|||2|1083660|||</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>FirstName</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>LastName</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>InsCardNo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CreateById</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>InsBenefitRatio</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>InsBenefitType</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1906</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Quách Bảo Hưng</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DN4127460129099</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>3839</v>
+      </c>
+      <c r="E2" t="n">
+        <v>80</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1907</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Quách Bảo Hưng</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>3839</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1908</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Quách Bảo Hưng</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>DN4127460129101</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3839</v>
+      </c>
+      <c r="E4" t="n">
+        <v>80</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1909</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Quách Bảo Hưng</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>3839</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>